<commit_message>
Commit search and bash script changes  - 24rd Sept
</commit_message>
<xml_diff>
--- a/invoices.xlsx
+++ b/invoices.xlsx
@@ -868,22 +868,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>SP23092022172048</t>
+          <t>SP23092022232857</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>100</v>
+        <v>280</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PANADOL STRIP 10</t>
+          <t>SIGMACORT CREAM 1% 50G</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E21" t="n">
-        <v>15</v>
+        <v>799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>